<commit_message>
second update loading doneclear
</commit_message>
<xml_diff>
--- a/assets/result.xlsx
+++ b/assets/result.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="154">
   <si>
     <t>Market</t>
   </si>
@@ -322,6 +322,9 @@
     <t>unlocked</t>
   </si>
   <si>
+    <t>700MHz</t>
+  </si>
+  <si>
     <t>AWS-1</t>
   </si>
   <si>
@@ -334,6 +337,9 @@
     <t>AWS3-1</t>
   </si>
   <si>
+    <t>CBRS</t>
+  </si>
+  <si>
     <t>10MHz</t>
   </si>
   <si>
@@ -343,25 +349,61 @@
     <t>15MHz</t>
   </si>
   <si>
+    <t>20MHz</t>
+  </si>
+  <si>
+    <t>cfg355-multi-carrier-10m-10m-10m-10m-5m-5m-5m-5m-config3</t>
+  </si>
+  <si>
     <t>cfg61-multi-carrier-10m-5m-6cell</t>
   </si>
   <si>
-    <t>cfg355-multi-carrier-10m-10m-10m-10m-5m-5m-5m-5m-config3</t>
-  </si>
-  <si>
     <t>cfg358-multi-carrier-20m-20m-20m-10m-5m-config3</t>
   </si>
   <si>
-    <t>181080_2_2;MC;ALLEN MORGAN TN</t>
-  </si>
-  <si>
-    <t>181080_2_4;MC;ALLEN MORGAN TN</t>
-  </si>
-  <si>
-    <t>181080_1_6;MC;ALLEN MORGAN TN</t>
-  </si>
-  <si>
-    <t>181080_2_8;MC;ALLEN MORGAN TN</t>
+    <t>181080_2;MC;ALLEN MORGAN TN</t>
+  </si>
+  <si>
+    <t>181080_3;MC;ALLEN MORGAN TN</t>
+  </si>
+  <si>
+    <t>181080_1_2;MC;ALLEN MORGAN TN</t>
+  </si>
+  <si>
+    <t>181080_3_2;MC;ALLEN MORGAN TN</t>
+  </si>
+  <si>
+    <t>181080_1_4;MC;ALLEN MORGAN TN</t>
+  </si>
+  <si>
+    <t>181080_3_4;MC;ALLEN MORGAN TN</t>
+  </si>
+  <si>
+    <t>181080_2_6;MC;ALLEN MORGAN TN</t>
+  </si>
+  <si>
+    <t>181080_3_6;MC;ALLEN MORGAN TN</t>
+  </si>
+  <si>
+    <t>181080_1_8;MC;ALLEN MORGAN TN</t>
+  </si>
+  <si>
+    <t>181080_3_8;MC;ALLEN MORGAN TN</t>
+  </si>
+  <si>
+    <t>181080_19;MC;ALLEN MORGAN TN</t>
+  </si>
+  <si>
+    <t>181080_19_2;MC;ALLEN MORGAN TN</t>
+  </si>
+  <si>
+    <t>181080_19_3;MC;ALLEN MORGAN TN</t>
+  </si>
+  <si>
+    <t>181080_19_4;MC;ALLEN MORGAN TN</t>
+  </si>
+  <si>
+    <t>181080_20;MC;ALLEN MORGAN TN</t>
   </si>
   <si>
     <t>ARTNTNBI</t>
@@ -376,6 +418,9 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
+    <t>QS8656-5_V3-0F_740MHZ_02DT_PORT1</t>
+  </si>
+  <si>
     <t>QS8656-5_V3-0F_2140MHZ_02DT_PORT3</t>
   </si>
   <si>
@@ -388,16 +433,25 @@
     <t>QS8610C4_V1-0P_2140MHz_02DT_Port3</t>
   </si>
   <si>
+    <t>QS8610C4_V1-0P_3600MHz_04DT_Port7</t>
+  </si>
+  <si>
+    <t>Samsung RRH (B5/B13 RRH ORAN )</t>
+  </si>
+  <si>
     <t>Samsung RRH (B2/B66A RRH ORAN )</t>
   </si>
   <si>
-    <t>Samsung RRH (B5/B13 RRH ORAN )</t>
+    <t>Samsung RRH (CBRS RRH)</t>
+  </si>
+  <si>
+    <t>Samsung RRH (RF4440d-13A)</t>
   </si>
   <si>
     <t>Samsung RRH (RF4439d-25A)</t>
   </si>
   <si>
-    <t>Samsung RRH (RF4440d-13A)</t>
+    <t>Samsung RRH (RT4401-48)</t>
   </si>
   <si>
     <t>No Type match</t>
@@ -407,6 +461,18 @@
   </si>
   <si>
     <t>911_ARTNTNBI_01_ABC</t>
+  </si>
+  <si>
+    <t>D0HBBA</t>
+  </si>
+  <si>
+    <t>A3LRT4401-48A</t>
+  </si>
+  <si>
+    <t>55990,56190,56390,56590</t>
+  </si>
+  <si>
+    <t>cbsd-b</t>
   </si>
   <si>
     <t>2001:5000:a45:3143:432:292::a100</t>
@@ -767,7 +833,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CR5"/>
+  <dimension ref="A1:CR16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1062,7 +1128,7 @@
     </row>
     <row r="2" spans="1:96">
       <c r="A2" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>95</v>
@@ -1080,16 +1146,16 @@
         <v>99</v>
       </c>
       <c r="H2">
-        <v>22</v>
+        <v>980181</v>
       </c>
       <c r="J2">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="K2" t="s">
         <v>100</v>
       </c>
       <c r="L2">
-        <v>46356502</v>
+        <v>46356482</v>
       </c>
       <c r="M2" t="s">
         <v>101</v>
@@ -1113,16 +1179,16 @@
         <v>102</v>
       </c>
       <c r="T2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="U2">
-        <v>2100</v>
+        <v>5230</v>
       </c>
       <c r="V2">
-        <v>20100</v>
+        <v>23230</v>
       </c>
       <c r="W2">
-        <v>47.7</v>
+        <v>46</v>
       </c>
       <c r="X2">
         <v>4</v>
@@ -1139,17 +1205,23 @@
       <c r="AB2">
         <v>120</v>
       </c>
+      <c r="AC2">
+        <v>1</v>
+      </c>
+      <c r="AD2">
+        <v>1</v>
+      </c>
       <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <v>0</v>
+      </c>
+      <c r="AH2">
         <v>1</v>
       </c>
-      <c r="AG2">
+      <c r="AI2">
         <v>1</v>
-      </c>
-      <c r="AH2">
-        <v>4</v>
-      </c>
-      <c r="AI2">
-        <v>4</v>
       </c>
       <c r="AK2">
         <v>0</v>
@@ -1164,13 +1236,13 @@
         <v>4</v>
       </c>
       <c r="AO2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="AP2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="AQ2" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
       <c r="AS2">
         <v>47157</v>
@@ -1179,48 +1251,48 @@
         <v>2</v>
       </c>
       <c r="AU2" t="s">
-        <v>117</v>
+        <v>131</v>
       </c>
       <c r="AV2">
         <v>0</v>
       </c>
       <c r="AW2" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="AX2" t="s">
-        <v>120</v>
+        <v>134</v>
       </c>
       <c r="AY2" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="AZ2" t="s">
-        <v>124</v>
+        <v>140</v>
       </c>
       <c r="BC2" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="BF2">
         <v>267466</v>
       </c>
       <c r="BG2" t="s">
-        <v>128</v>
+        <v>146</v>
       </c>
       <c r="BM2" t="s">
-        <v>129</v>
+        <v>147</v>
       </c>
       <c r="BR2" t="s">
-        <v>130</v>
+        <v>148</v>
       </c>
       <c r="BZ2">
         <v>39396</v>
       </c>
       <c r="CL2" t="s">
-        <v>131</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:96">
       <c r="A3" s="1">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>95</v>
@@ -1238,16 +1310,16 @@
         <v>99</v>
       </c>
       <c r="H3">
-        <v>22</v>
+        <v>980181</v>
       </c>
       <c r="J3">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="K3" t="s">
         <v>100</v>
       </c>
       <c r="L3">
-        <v>46356504</v>
+        <v>46356483</v>
       </c>
       <c r="M3" t="s">
         <v>101</v>
@@ -1262,25 +1334,25 @@
         <v>46344</v>
       </c>
       <c r="Q3">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="R3">
         <v>170</v>
       </c>
       <c r="S3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="T3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="U3">
-        <v>975</v>
+        <v>5230</v>
       </c>
       <c r="V3">
-        <v>18975</v>
+        <v>23230</v>
       </c>
       <c r="W3">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="X3">
         <v>4</v>
@@ -1295,19 +1367,25 @@
         <v>29.5</v>
       </c>
       <c r="AB3">
-        <v>120</v>
+        <v>240</v>
+      </c>
+      <c r="AC3">
+        <v>1</v>
+      </c>
+      <c r="AD3">
+        <v>1</v>
       </c>
       <c r="AF3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AK3">
         <v>0</v>
@@ -1316,19 +1394,19 @@
         <v>12</v>
       </c>
       <c r="AM3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AN3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AO3" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="AP3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="AQ3" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
       <c r="AS3">
         <v>47157</v>
@@ -1337,48 +1415,48 @@
         <v>2</v>
       </c>
       <c r="AU3" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="AV3">
         <v>0</v>
       </c>
       <c r="AW3" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="AX3" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
       <c r="AY3" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="AZ3" t="s">
-        <v>124</v>
+        <v>140</v>
       </c>
       <c r="BC3" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="BF3">
         <v>267466</v>
       </c>
       <c r="BG3" t="s">
-        <v>128</v>
+        <v>146</v>
       </c>
       <c r="BM3" t="s">
-        <v>129</v>
+        <v>147</v>
       </c>
       <c r="BR3" t="s">
-        <v>130</v>
+        <v>148</v>
       </c>
       <c r="BZ3">
         <v>39396</v>
       </c>
       <c r="CL3" t="s">
-        <v>131</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:96">
       <c r="A4" s="1">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>95</v>
@@ -1396,16 +1474,16 @@
         <v>99</v>
       </c>
       <c r="H4">
-        <v>22</v>
+        <v>980181</v>
       </c>
       <c r="J4">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="K4" t="s">
         <v>100</v>
       </c>
       <c r="L4">
-        <v>46356496</v>
+        <v>46356492</v>
       </c>
       <c r="M4" t="s">
         <v>101</v>
@@ -1426,19 +1504,19 @@
         <v>170</v>
       </c>
       <c r="S4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="T4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="U4">
-        <v>2450</v>
+        <v>2100</v>
       </c>
       <c r="V4">
-        <v>20450</v>
+        <v>20100</v>
       </c>
       <c r="W4">
-        <v>43</v>
+        <v>47.7</v>
       </c>
       <c r="X4">
         <v>4</v>
@@ -1456,16 +1534,16 @@
         <v>0</v>
       </c>
       <c r="AF4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG4">
         <v>1</v>
       </c>
       <c r="AH4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AI4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AK4">
         <v>0</v>
@@ -1480,13 +1558,13 @@
         <v>3</v>
       </c>
       <c r="AO4" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="AP4" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AQ4" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
       <c r="AS4">
         <v>47157</v>
@@ -1495,48 +1573,48 @@
         <v>2</v>
       </c>
       <c r="AU4" t="s">
-        <v>117</v>
+        <v>131</v>
       </c>
       <c r="AV4">
         <v>0</v>
       </c>
       <c r="AW4" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="AX4" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="AY4" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="AZ4" t="s">
-        <v>125</v>
+        <v>141</v>
       </c>
       <c r="BC4" t="s">
-        <v>127</v>
+        <v>144</v>
       </c>
       <c r="BF4">
         <v>267466</v>
       </c>
       <c r="BG4" t="s">
-        <v>128</v>
+        <v>146</v>
       </c>
       <c r="BM4" t="s">
-        <v>129</v>
+        <v>147</v>
       </c>
       <c r="BR4" t="s">
-        <v>130</v>
+        <v>148</v>
       </c>
       <c r="BZ4">
         <v>39396</v>
       </c>
       <c r="CL4" t="s">
-        <v>131</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:96">
       <c r="A5" s="1">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>95</v>
@@ -1554,16 +1632,16 @@
         <v>99</v>
       </c>
       <c r="H5">
-        <v>22</v>
+        <v>980181</v>
       </c>
       <c r="J5">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="K5" t="s">
         <v>100</v>
       </c>
       <c r="L5">
-        <v>46356508</v>
+        <v>46356512</v>
       </c>
       <c r="M5" t="s">
         <v>101</v>
@@ -1578,22 +1656,22 @@
         <v>46344</v>
       </c>
       <c r="Q5">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="R5">
         <v>170</v>
       </c>
       <c r="S5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="T5" t="s">
         <v>108</v>
       </c>
       <c r="U5">
-        <v>66911</v>
+        <v>2100</v>
       </c>
       <c r="V5">
-        <v>132447</v>
+        <v>20100</v>
       </c>
       <c r="W5">
         <v>47.7</v>
@@ -1611,40 +1689,40 @@
         <v>29.5</v>
       </c>
       <c r="AB5">
-        <v>120</v>
+        <v>240</v>
       </c>
       <c r="AF5">
         <v>1</v>
       </c>
       <c r="AG5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AI5">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="AK5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL5">
         <v>12</v>
       </c>
       <c r="AM5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AN5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AO5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="AP5" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="AQ5" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
       <c r="AS5">
         <v>47157</v>
@@ -1653,43 +1731,1931 @@
         <v>2</v>
       </c>
       <c r="AU5" t="s">
-        <v>117</v>
+        <v>131</v>
       </c>
       <c r="AV5">
         <v>0</v>
       </c>
       <c r="AW5" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="AX5" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="AY5" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="AZ5" t="s">
-        <v>124</v>
+        <v>141</v>
       </c>
       <c r="BC5" t="s">
-        <v>126</v>
+        <v>144</v>
       </c>
       <c r="BF5">
         <v>267466</v>
       </c>
       <c r="BG5" t="s">
-        <v>128</v>
+        <v>146</v>
       </c>
       <c r="BM5" t="s">
-        <v>129</v>
+        <v>147</v>
       </c>
       <c r="BR5" t="s">
-        <v>130</v>
+        <v>148</v>
       </c>
       <c r="BZ5">
         <v>39396</v>
       </c>
       <c r="CL5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="1:96">
+      <c r="A6" s="1">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D6" t="s">
+        <v>97</v>
+      </c>
+      <c r="E6" t="s">
+        <v>98</v>
+      </c>
+      <c r="F6" t="s">
+        <v>99</v>
+      </c>
+      <c r="H6">
+        <v>980181</v>
+      </c>
+      <c r="J6">
+        <v>14</v>
+      </c>
+      <c r="K6" t="s">
+        <v>100</v>
+      </c>
+      <c r="L6">
+        <v>46356494</v>
+      </c>
+      <c r="M6" t="s">
+        <v>101</v>
+      </c>
+      <c r="N6">
+        <v>35.136722</v>
+      </c>
+      <c r="O6">
+        <v>-89.945753</v>
+      </c>
+      <c r="P6">
+        <v>46344</v>
+      </c>
+      <c r="Q6">
+        <v>201</v>
+      </c>
+      <c r="R6">
+        <v>170</v>
+      </c>
+      <c r="S6" t="s">
+        <v>104</v>
+      </c>
+      <c r="T6" t="s">
+        <v>109</v>
+      </c>
+      <c r="U6">
+        <v>975</v>
+      </c>
+      <c r="V6">
+        <v>18975</v>
+      </c>
+      <c r="W6">
+        <v>43</v>
+      </c>
+      <c r="X6">
+        <v>4</v>
+      </c>
+      <c r="Y6">
+        <v>4</v>
+      </c>
+      <c r="Z6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA6">
+        <v>29.5</v>
+      </c>
+      <c r="AB6">
+        <v>0</v>
+      </c>
+      <c r="AF6">
+        <v>1</v>
+      </c>
+      <c r="AG6">
+        <v>1</v>
+      </c>
+      <c r="AH6">
+        <v>0</v>
+      </c>
+      <c r="AI6">
+        <v>3</v>
+      </c>
+      <c r="AK6">
+        <v>0</v>
+      </c>
+      <c r="AL6">
+        <v>12</v>
+      </c>
+      <c r="AM6">
+        <v>3</v>
+      </c>
+      <c r="AN6">
+        <v>3</v>
+      </c>
+      <c r="AO6" t="s">
+        <v>113</v>
+      </c>
+      <c r="AP6" t="s">
+        <v>119</v>
+      </c>
+      <c r="AQ6" t="s">
+        <v>130</v>
+      </c>
+      <c r="AS6">
+        <v>47157</v>
+      </c>
+      <c r="AT6">
+        <v>2</v>
+      </c>
+      <c r="AU6" t="s">
+        <v>132</v>
+      </c>
+      <c r="AV6">
+        <v>0</v>
+      </c>
+      <c r="AW6" t="s">
+        <v>133</v>
+      </c>
+      <c r="AX6" t="s">
+        <v>136</v>
+      </c>
+      <c r="AY6" t="s">
+        <v>133</v>
+      </c>
+      <c r="AZ6" t="s">
+        <v>141</v>
+      </c>
+      <c r="BC6" t="s">
+        <v>144</v>
+      </c>
+      <c r="BF6">
+        <v>267466</v>
+      </c>
+      <c r="BG6" t="s">
+        <v>146</v>
+      </c>
+      <c r="BM6" t="s">
+        <v>147</v>
+      </c>
+      <c r="BR6" t="s">
+        <v>148</v>
+      </c>
+      <c r="BZ6">
+        <v>39396</v>
+      </c>
+      <c r="CL6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:96">
+      <c r="A7" s="1">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D7" t="s">
+        <v>97</v>
+      </c>
+      <c r="E7" t="s">
+        <v>98</v>
+      </c>
+      <c r="F7" t="s">
+        <v>99</v>
+      </c>
+      <c r="H7">
+        <v>980181</v>
+      </c>
+      <c r="J7">
+        <v>34</v>
+      </c>
+      <c r="K7" t="s">
+        <v>100</v>
+      </c>
+      <c r="L7">
+        <v>46356514</v>
+      </c>
+      <c r="M7" t="s">
+        <v>101</v>
+      </c>
+      <c r="N7">
+        <v>35.136722</v>
+      </c>
+      <c r="O7">
+        <v>-89.945753</v>
+      </c>
+      <c r="P7">
+        <v>46344</v>
+      </c>
+      <c r="Q7">
+        <v>203</v>
+      </c>
+      <c r="R7">
+        <v>170</v>
+      </c>
+      <c r="S7" t="s">
+        <v>104</v>
+      </c>
+      <c r="T7" t="s">
+        <v>109</v>
+      </c>
+      <c r="U7">
+        <v>975</v>
+      </c>
+      <c r="V7">
+        <v>18975</v>
+      </c>
+      <c r="W7">
+        <v>43</v>
+      </c>
+      <c r="X7">
+        <v>4</v>
+      </c>
+      <c r="Y7">
+        <v>4</v>
+      </c>
+      <c r="Z7" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA7">
+        <v>29.5</v>
+      </c>
+      <c r="AB7">
+        <v>240</v>
+      </c>
+      <c r="AF7">
+        <v>1</v>
+      </c>
+      <c r="AG7">
+        <v>1</v>
+      </c>
+      <c r="AH7">
+        <v>2</v>
+      </c>
+      <c r="AI7">
+        <v>5</v>
+      </c>
+      <c r="AK7">
+        <v>0</v>
+      </c>
+      <c r="AL7">
+        <v>12</v>
+      </c>
+      <c r="AM7">
+        <v>5</v>
+      </c>
+      <c r="AN7">
+        <v>5</v>
+      </c>
+      <c r="AO7" t="s">
+        <v>113</v>
+      </c>
+      <c r="AP7" t="s">
+        <v>120</v>
+      </c>
+      <c r="AQ7" t="s">
+        <v>130</v>
+      </c>
+      <c r="AS7">
+        <v>47157</v>
+      </c>
+      <c r="AT7">
+        <v>2</v>
+      </c>
+      <c r="AU7" t="s">
+        <v>132</v>
+      </c>
+      <c r="AV7">
+        <v>0</v>
+      </c>
+      <c r="AW7" t="s">
+        <v>133</v>
+      </c>
+      <c r="AX7" t="s">
+        <v>136</v>
+      </c>
+      <c r="AY7" t="s">
+        <v>133</v>
+      </c>
+      <c r="AZ7" t="s">
+        <v>141</v>
+      </c>
+      <c r="BC7" t="s">
+        <v>144</v>
+      </c>
+      <c r="BF7">
+        <v>267466</v>
+      </c>
+      <c r="BG7" t="s">
+        <v>146</v>
+      </c>
+      <c r="BM7" t="s">
+        <v>147</v>
+      </c>
+      <c r="BR7" t="s">
+        <v>148</v>
+      </c>
+      <c r="BZ7">
+        <v>39396</v>
+      </c>
+      <c r="CL7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:96">
+      <c r="A8" s="1">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" t="s">
+        <v>97</v>
+      </c>
+      <c r="E8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F8" t="s">
+        <v>99</v>
+      </c>
+      <c r="H8">
+        <v>980181</v>
+      </c>
+      <c r="J8">
+        <v>26</v>
+      </c>
+      <c r="K8" t="s">
+        <v>100</v>
+      </c>
+      <c r="L8">
+        <v>46356506</v>
+      </c>
+      <c r="M8" t="s">
+        <v>101</v>
+      </c>
+      <c r="N8">
+        <v>35.136722</v>
+      </c>
+      <c r="O8">
+        <v>-89.945753</v>
+      </c>
+      <c r="P8">
+        <v>46344</v>
+      </c>
+      <c r="Q8">
+        <v>202</v>
+      </c>
+      <c r="R8">
+        <v>170</v>
+      </c>
+      <c r="S8" t="s">
+        <v>105</v>
+      </c>
+      <c r="T8" t="s">
+        <v>108</v>
+      </c>
+      <c r="U8">
+        <v>2450</v>
+      </c>
+      <c r="V8">
+        <v>20450</v>
+      </c>
+      <c r="W8">
+        <v>43</v>
+      </c>
+      <c r="X8">
+        <v>4</v>
+      </c>
+      <c r="Y8">
+        <v>4</v>
+      </c>
+      <c r="Z8" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA8">
+        <v>29.5</v>
+      </c>
+      <c r="AB8">
+        <v>120</v>
+      </c>
+      <c r="AF8">
+        <v>0</v>
+      </c>
+      <c r="AG8">
+        <v>1</v>
+      </c>
+      <c r="AH8">
+        <v>1</v>
+      </c>
+      <c r="AI8">
+        <v>1</v>
+      </c>
+      <c r="AK8">
+        <v>0</v>
+      </c>
+      <c r="AL8">
+        <v>12</v>
+      </c>
+      <c r="AM8">
+        <v>4</v>
+      </c>
+      <c r="AN8">
+        <v>4</v>
+      </c>
+      <c r="AO8" t="s">
+        <v>112</v>
+      </c>
+      <c r="AP8" t="s">
+        <v>121</v>
+      </c>
+      <c r="AQ8" t="s">
+        <v>130</v>
+      </c>
+      <c r="AS8">
+        <v>47157</v>
+      </c>
+      <c r="AT8">
+        <v>2</v>
+      </c>
+      <c r="AU8" t="s">
         <v>131</v>
+      </c>
+      <c r="AV8">
+        <v>0</v>
+      </c>
+      <c r="AW8" t="s">
+        <v>133</v>
+      </c>
+      <c r="AX8" t="s">
+        <v>137</v>
+      </c>
+      <c r="AY8" t="s">
+        <v>133</v>
+      </c>
+      <c r="AZ8" t="s">
+        <v>140</v>
+      </c>
+      <c r="BC8" t="s">
+        <v>143</v>
+      </c>
+      <c r="BF8">
+        <v>267466</v>
+      </c>
+      <c r="BG8" t="s">
+        <v>146</v>
+      </c>
+      <c r="BM8" t="s">
+        <v>147</v>
+      </c>
+      <c r="BR8" t="s">
+        <v>148</v>
+      </c>
+      <c r="BZ8">
+        <v>39396</v>
+      </c>
+      <c r="CL8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:96">
+      <c r="A9" s="1">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E9" t="s">
+        <v>98</v>
+      </c>
+      <c r="F9" t="s">
+        <v>99</v>
+      </c>
+      <c r="H9">
+        <v>980181</v>
+      </c>
+      <c r="J9">
+        <v>36</v>
+      </c>
+      <c r="K9" t="s">
+        <v>100</v>
+      </c>
+      <c r="L9">
+        <v>46356516</v>
+      </c>
+      <c r="M9" t="s">
+        <v>101</v>
+      </c>
+      <c r="N9">
+        <v>35.136722</v>
+      </c>
+      <c r="O9">
+        <v>-89.945753</v>
+      </c>
+      <c r="P9">
+        <v>46344</v>
+      </c>
+      <c r="Q9">
+        <v>203</v>
+      </c>
+      <c r="R9">
+        <v>170</v>
+      </c>
+      <c r="S9" t="s">
+        <v>105</v>
+      </c>
+      <c r="T9" t="s">
+        <v>108</v>
+      </c>
+      <c r="U9">
+        <v>2450</v>
+      </c>
+      <c r="V9">
+        <v>20450</v>
+      </c>
+      <c r="W9">
+        <v>43</v>
+      </c>
+      <c r="X9">
+        <v>4</v>
+      </c>
+      <c r="Y9">
+        <v>4</v>
+      </c>
+      <c r="Z9" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA9">
+        <v>29.5</v>
+      </c>
+      <c r="AB9">
+        <v>240</v>
+      </c>
+      <c r="AF9">
+        <v>0</v>
+      </c>
+      <c r="AG9">
+        <v>1</v>
+      </c>
+      <c r="AH9">
+        <v>2</v>
+      </c>
+      <c r="AI9">
+        <v>2</v>
+      </c>
+      <c r="AK9">
+        <v>0</v>
+      </c>
+      <c r="AL9">
+        <v>12</v>
+      </c>
+      <c r="AM9">
+        <v>5</v>
+      </c>
+      <c r="AN9">
+        <v>5</v>
+      </c>
+      <c r="AO9" t="s">
+        <v>112</v>
+      </c>
+      <c r="AP9" t="s">
+        <v>122</v>
+      </c>
+      <c r="AQ9" t="s">
+        <v>130</v>
+      </c>
+      <c r="AS9">
+        <v>47157</v>
+      </c>
+      <c r="AT9">
+        <v>2</v>
+      </c>
+      <c r="AU9" t="s">
+        <v>131</v>
+      </c>
+      <c r="AV9">
+        <v>0</v>
+      </c>
+      <c r="AW9" t="s">
+        <v>133</v>
+      </c>
+      <c r="AX9" t="s">
+        <v>137</v>
+      </c>
+      <c r="AY9" t="s">
+        <v>133</v>
+      </c>
+      <c r="AZ9" t="s">
+        <v>140</v>
+      </c>
+      <c r="BC9" t="s">
+        <v>143</v>
+      </c>
+      <c r="BF9">
+        <v>267466</v>
+      </c>
+      <c r="BG9" t="s">
+        <v>146</v>
+      </c>
+      <c r="BM9" t="s">
+        <v>147</v>
+      </c>
+      <c r="BR9" t="s">
+        <v>148</v>
+      </c>
+      <c r="BZ9">
+        <v>39396</v>
+      </c>
+      <c r="CL9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="10" spans="1:96">
+      <c r="A10" s="1">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" t="s">
+        <v>98</v>
+      </c>
+      <c r="F10" t="s">
+        <v>99</v>
+      </c>
+      <c r="H10">
+        <v>980181</v>
+      </c>
+      <c r="J10">
+        <v>18</v>
+      </c>
+      <c r="K10" t="s">
+        <v>100</v>
+      </c>
+      <c r="L10">
+        <v>46356498</v>
+      </c>
+      <c r="M10" t="s">
+        <v>101</v>
+      </c>
+      <c r="N10">
+        <v>35.136722</v>
+      </c>
+      <c r="O10">
+        <v>-89.945753</v>
+      </c>
+      <c r="P10">
+        <v>46344</v>
+      </c>
+      <c r="Q10">
+        <v>201</v>
+      </c>
+      <c r="R10">
+        <v>170</v>
+      </c>
+      <c r="S10" t="s">
+        <v>106</v>
+      </c>
+      <c r="T10" t="s">
+        <v>110</v>
+      </c>
+      <c r="U10">
+        <v>66911</v>
+      </c>
+      <c r="V10">
+        <v>132447</v>
+      </c>
+      <c r="W10">
+        <v>47.7</v>
+      </c>
+      <c r="X10">
+        <v>4</v>
+      </c>
+      <c r="Y10">
+        <v>4</v>
+      </c>
+      <c r="Z10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA10">
+        <v>29.5</v>
+      </c>
+      <c r="AB10">
+        <v>0</v>
+      </c>
+      <c r="AF10">
+        <v>1</v>
+      </c>
+      <c r="AG10">
+        <v>0</v>
+      </c>
+      <c r="AH10">
+        <v>0</v>
+      </c>
+      <c r="AI10">
+        <v>6</v>
+      </c>
+      <c r="AK10">
+        <v>1</v>
+      </c>
+      <c r="AL10">
+        <v>12</v>
+      </c>
+      <c r="AM10">
+        <v>3</v>
+      </c>
+      <c r="AN10">
+        <v>3</v>
+      </c>
+      <c r="AO10" t="s">
+        <v>114</v>
+      </c>
+      <c r="AP10" t="s">
+        <v>123</v>
+      </c>
+      <c r="AQ10" t="s">
+        <v>130</v>
+      </c>
+      <c r="AS10">
+        <v>47157</v>
+      </c>
+      <c r="AT10">
+        <v>2</v>
+      </c>
+      <c r="AU10" t="s">
+        <v>131</v>
+      </c>
+      <c r="AV10">
+        <v>0</v>
+      </c>
+      <c r="AW10" t="s">
+        <v>133</v>
+      </c>
+      <c r="AX10" t="s">
+        <v>138</v>
+      </c>
+      <c r="AY10" t="s">
+        <v>133</v>
+      </c>
+      <c r="AZ10" t="s">
+        <v>141</v>
+      </c>
+      <c r="BC10" t="s">
+        <v>144</v>
+      </c>
+      <c r="BF10">
+        <v>267466</v>
+      </c>
+      <c r="BG10" t="s">
+        <v>146</v>
+      </c>
+      <c r="BM10" t="s">
+        <v>147</v>
+      </c>
+      <c r="BR10" t="s">
+        <v>148</v>
+      </c>
+      <c r="BZ10">
+        <v>39396</v>
+      </c>
+      <c r="CL10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:96">
+      <c r="A11" s="1">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" t="s">
+        <v>96</v>
+      </c>
+      <c r="D11" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11" t="s">
+        <v>98</v>
+      </c>
+      <c r="F11" t="s">
+        <v>99</v>
+      </c>
+      <c r="H11">
+        <v>980181</v>
+      </c>
+      <c r="J11">
+        <v>38</v>
+      </c>
+      <c r="K11" t="s">
+        <v>100</v>
+      </c>
+      <c r="L11">
+        <v>46356518</v>
+      </c>
+      <c r="M11" t="s">
+        <v>101</v>
+      </c>
+      <c r="N11">
+        <v>35.136722</v>
+      </c>
+      <c r="O11">
+        <v>-89.945753</v>
+      </c>
+      <c r="P11">
+        <v>46344</v>
+      </c>
+      <c r="Q11">
+        <v>203</v>
+      </c>
+      <c r="R11">
+        <v>170</v>
+      </c>
+      <c r="S11" t="s">
+        <v>106</v>
+      </c>
+      <c r="T11" t="s">
+        <v>110</v>
+      </c>
+      <c r="U11">
+        <v>66911</v>
+      </c>
+      <c r="V11">
+        <v>132447</v>
+      </c>
+      <c r="W11">
+        <v>47.7</v>
+      </c>
+      <c r="X11">
+        <v>4</v>
+      </c>
+      <c r="Y11">
+        <v>4</v>
+      </c>
+      <c r="Z11" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA11">
+        <v>29.5</v>
+      </c>
+      <c r="AB11">
+        <v>240</v>
+      </c>
+      <c r="AF11">
+        <v>1</v>
+      </c>
+      <c r="AG11">
+        <v>0</v>
+      </c>
+      <c r="AH11">
+        <v>2</v>
+      </c>
+      <c r="AI11">
+        <v>8</v>
+      </c>
+      <c r="AK11">
+        <v>1</v>
+      </c>
+      <c r="AL11">
+        <v>12</v>
+      </c>
+      <c r="AM11">
+        <v>5</v>
+      </c>
+      <c r="AN11">
+        <v>5</v>
+      </c>
+      <c r="AO11" t="s">
+        <v>114</v>
+      </c>
+      <c r="AP11" t="s">
+        <v>124</v>
+      </c>
+      <c r="AQ11" t="s">
+        <v>130</v>
+      </c>
+      <c r="AS11">
+        <v>47157</v>
+      </c>
+      <c r="AT11">
+        <v>2</v>
+      </c>
+      <c r="AU11" t="s">
+        <v>131</v>
+      </c>
+      <c r="AV11">
+        <v>0</v>
+      </c>
+      <c r="AW11" t="s">
+        <v>133</v>
+      </c>
+      <c r="AX11" t="s">
+        <v>138</v>
+      </c>
+      <c r="AY11" t="s">
+        <v>133</v>
+      </c>
+      <c r="AZ11" t="s">
+        <v>141</v>
+      </c>
+      <c r="BC11" t="s">
+        <v>144</v>
+      </c>
+      <c r="BF11">
+        <v>267466</v>
+      </c>
+      <c r="BG11" t="s">
+        <v>146</v>
+      </c>
+      <c r="BM11" t="s">
+        <v>147</v>
+      </c>
+      <c r="BR11" t="s">
+        <v>148</v>
+      </c>
+      <c r="BZ11">
+        <v>39396</v>
+      </c>
+      <c r="CL11" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="12" spans="1:96">
+      <c r="A12" s="1">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C12" t="s">
+        <v>96</v>
+      </c>
+      <c r="D12" t="s">
+        <v>97</v>
+      </c>
+      <c r="E12" t="s">
+        <v>98</v>
+      </c>
+      <c r="F12" t="s">
+        <v>99</v>
+      </c>
+      <c r="H12">
+        <v>980181</v>
+      </c>
+      <c r="J12">
+        <v>191</v>
+      </c>
+      <c r="K12" t="s">
+        <v>100</v>
+      </c>
+      <c r="L12">
+        <v>46356671</v>
+      </c>
+      <c r="M12" t="s">
+        <v>101</v>
+      </c>
+      <c r="N12">
+        <v>35.136722</v>
+      </c>
+      <c r="O12">
+        <v>-89.945753</v>
+      </c>
+      <c r="P12">
+        <v>46344</v>
+      </c>
+      <c r="Q12">
+        <v>201</v>
+      </c>
+      <c r="R12">
+        <v>170</v>
+      </c>
+      <c r="S12" t="s">
+        <v>107</v>
+      </c>
+      <c r="T12" t="s">
+        <v>108</v>
+      </c>
+      <c r="U12">
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>30.9</v>
+      </c>
+      <c r="X12">
+        <v>4</v>
+      </c>
+      <c r="Y12">
+        <v>4</v>
+      </c>
+      <c r="Z12" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA12">
+        <v>29.5</v>
+      </c>
+      <c r="AB12">
+        <v>0</v>
+      </c>
+      <c r="AF12">
+        <v>2</v>
+      </c>
+      <c r="AG12">
+        <v>0</v>
+      </c>
+      <c r="AH12">
+        <v>0</v>
+      </c>
+      <c r="AI12">
+        <v>6</v>
+      </c>
+      <c r="AJ12">
+        <v>6</v>
+      </c>
+      <c r="AK12">
+        <v>0</v>
+      </c>
+      <c r="AL12">
+        <v>12</v>
+      </c>
+      <c r="AM12">
+        <v>3</v>
+      </c>
+      <c r="AN12">
+        <v>3</v>
+      </c>
+      <c r="AO12" t="s">
+        <v>114</v>
+      </c>
+      <c r="AP12" t="s">
+        <v>125</v>
+      </c>
+      <c r="AQ12" t="s">
+        <v>130</v>
+      </c>
+      <c r="AS12">
+        <v>47157</v>
+      </c>
+      <c r="AT12">
+        <v>4</v>
+      </c>
+      <c r="AU12" t="s">
+        <v>131</v>
+      </c>
+      <c r="AV12">
+        <v>0</v>
+      </c>
+      <c r="AW12" t="s">
+        <v>133</v>
+      </c>
+      <c r="AX12" t="s">
+        <v>139</v>
+      </c>
+      <c r="AY12" t="s">
+        <v>133</v>
+      </c>
+      <c r="AZ12" t="s">
+        <v>142</v>
+      </c>
+      <c r="BC12" t="s">
+        <v>145</v>
+      </c>
+      <c r="BF12">
+        <v>267466</v>
+      </c>
+      <c r="BG12" t="s">
+        <v>146</v>
+      </c>
+      <c r="BM12" t="s">
+        <v>147</v>
+      </c>
+      <c r="BR12" t="s">
+        <v>148</v>
+      </c>
+      <c r="BZ12">
+        <v>39396</v>
+      </c>
+      <c r="CB12">
+        <v>0</v>
+      </c>
+      <c r="CC12">
+        <v>0</v>
+      </c>
+      <c r="CD12" t="s">
+        <v>149</v>
+      </c>
+      <c r="CE12" t="s">
+        <v>150</v>
+      </c>
+      <c r="CG12">
+        <v>37</v>
+      </c>
+      <c r="CH12" t="s">
+        <v>151</v>
+      </c>
+      <c r="CI12" t="s">
+        <v>152</v>
+      </c>
+      <c r="CJ12" t="b">
+        <v>1</v>
+      </c>
+      <c r="CK12">
+        <v>13.148</v>
+      </c>
+      <c r="CL12" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:96">
+      <c r="A13" s="1">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C13" t="s">
+        <v>96</v>
+      </c>
+      <c r="D13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E13" t="s">
+        <v>98</v>
+      </c>
+      <c r="F13" t="s">
+        <v>99</v>
+      </c>
+      <c r="H13">
+        <v>980181</v>
+      </c>
+      <c r="J13">
+        <v>192</v>
+      </c>
+      <c r="K13" t="s">
+        <v>100</v>
+      </c>
+      <c r="L13">
+        <v>46356672</v>
+      </c>
+      <c r="M13" t="s">
+        <v>101</v>
+      </c>
+      <c r="N13">
+        <v>35.136722</v>
+      </c>
+      <c r="O13">
+        <v>-89.945753</v>
+      </c>
+      <c r="P13">
+        <v>46344</v>
+      </c>
+      <c r="Q13">
+        <v>201</v>
+      </c>
+      <c r="R13">
+        <v>170</v>
+      </c>
+      <c r="S13" t="s">
+        <v>107</v>
+      </c>
+      <c r="T13" t="s">
+        <v>111</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <v>30.9</v>
+      </c>
+      <c r="X13">
+        <v>4</v>
+      </c>
+      <c r="Y13">
+        <v>4</v>
+      </c>
+      <c r="Z13" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA13">
+        <v>29.5</v>
+      </c>
+      <c r="AB13">
+        <v>0</v>
+      </c>
+      <c r="AF13">
+        <v>2</v>
+      </c>
+      <c r="AG13">
+        <v>0</v>
+      </c>
+      <c r="AH13">
+        <v>1</v>
+      </c>
+      <c r="AI13">
+        <v>6</v>
+      </c>
+      <c r="AJ13">
+        <v>6</v>
+      </c>
+      <c r="AK13">
+        <v>1</v>
+      </c>
+      <c r="AL13">
+        <v>12</v>
+      </c>
+      <c r="AM13">
+        <v>3</v>
+      </c>
+      <c r="AN13">
+        <v>3</v>
+      </c>
+      <c r="AO13" t="s">
+        <v>114</v>
+      </c>
+      <c r="AP13" t="s">
+        <v>126</v>
+      </c>
+      <c r="AQ13" t="s">
+        <v>130</v>
+      </c>
+      <c r="AS13">
+        <v>47157</v>
+      </c>
+      <c r="AT13">
+        <v>4</v>
+      </c>
+      <c r="AU13" t="s">
+        <v>131</v>
+      </c>
+      <c r="AV13">
+        <v>0</v>
+      </c>
+      <c r="AW13" t="s">
+        <v>133</v>
+      </c>
+      <c r="AX13" t="s">
+        <v>139</v>
+      </c>
+      <c r="AY13" t="s">
+        <v>133</v>
+      </c>
+      <c r="AZ13" t="s">
+        <v>142</v>
+      </c>
+      <c r="BC13" t="s">
+        <v>145</v>
+      </c>
+      <c r="BF13">
+        <v>267466</v>
+      </c>
+      <c r="BG13" t="s">
+        <v>146</v>
+      </c>
+      <c r="BM13" t="s">
+        <v>147</v>
+      </c>
+      <c r="BR13" t="s">
+        <v>148</v>
+      </c>
+      <c r="BZ13">
+        <v>39396</v>
+      </c>
+      <c r="CB13">
+        <v>0</v>
+      </c>
+      <c r="CC13">
+        <v>1</v>
+      </c>
+      <c r="CD13" t="s">
+        <v>149</v>
+      </c>
+      <c r="CE13" t="s">
+        <v>150</v>
+      </c>
+      <c r="CG13">
+        <v>37</v>
+      </c>
+      <c r="CH13" t="s">
+        <v>151</v>
+      </c>
+      <c r="CI13" t="s">
+        <v>152</v>
+      </c>
+      <c r="CJ13" t="b">
+        <v>1</v>
+      </c>
+      <c r="CK13">
+        <v>13.148</v>
+      </c>
+      <c r="CL13" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="14" spans="1:96">
+      <c r="A14" s="1">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D14" t="s">
+        <v>97</v>
+      </c>
+      <c r="E14" t="s">
+        <v>98</v>
+      </c>
+      <c r="F14" t="s">
+        <v>99</v>
+      </c>
+      <c r="H14">
+        <v>980181</v>
+      </c>
+      <c r="J14">
+        <v>193</v>
+      </c>
+      <c r="K14" t="s">
+        <v>100</v>
+      </c>
+      <c r="L14">
+        <v>46356673</v>
+      </c>
+      <c r="M14" t="s">
+        <v>101</v>
+      </c>
+      <c r="N14">
+        <v>35.136722</v>
+      </c>
+      <c r="O14">
+        <v>-89.945753</v>
+      </c>
+      <c r="P14">
+        <v>46344</v>
+      </c>
+      <c r="Q14">
+        <v>201</v>
+      </c>
+      <c r="R14">
+        <v>170</v>
+      </c>
+      <c r="S14" t="s">
+        <v>107</v>
+      </c>
+      <c r="T14" t="s">
+        <v>111</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <v>30.9</v>
+      </c>
+      <c r="X14">
+        <v>4</v>
+      </c>
+      <c r="Y14">
+        <v>4</v>
+      </c>
+      <c r="Z14" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA14">
+        <v>29.5</v>
+      </c>
+      <c r="AB14">
+        <v>0</v>
+      </c>
+      <c r="AF14">
+        <v>2</v>
+      </c>
+      <c r="AG14">
+        <v>0</v>
+      </c>
+      <c r="AH14">
+        <v>2</v>
+      </c>
+      <c r="AI14">
+        <v>7</v>
+      </c>
+      <c r="AJ14">
+        <v>6</v>
+      </c>
+      <c r="AK14">
+        <v>1</v>
+      </c>
+      <c r="AL14">
+        <v>12</v>
+      </c>
+      <c r="AM14">
+        <v>3</v>
+      </c>
+      <c r="AN14">
+        <v>3</v>
+      </c>
+      <c r="AO14" t="s">
+        <v>114</v>
+      </c>
+      <c r="AP14" t="s">
+        <v>127</v>
+      </c>
+      <c r="AQ14" t="s">
+        <v>130</v>
+      </c>
+      <c r="AS14">
+        <v>47157</v>
+      </c>
+      <c r="AT14">
+        <v>4</v>
+      </c>
+      <c r="AU14" t="s">
+        <v>131</v>
+      </c>
+      <c r="AV14">
+        <v>0</v>
+      </c>
+      <c r="AW14" t="s">
+        <v>133</v>
+      </c>
+      <c r="AX14" t="s">
+        <v>139</v>
+      </c>
+      <c r="AY14" t="s">
+        <v>133</v>
+      </c>
+      <c r="AZ14" t="s">
+        <v>142</v>
+      </c>
+      <c r="BC14" t="s">
+        <v>145</v>
+      </c>
+      <c r="BF14">
+        <v>267466</v>
+      </c>
+      <c r="BG14" t="s">
+        <v>146</v>
+      </c>
+      <c r="BM14" t="s">
+        <v>147</v>
+      </c>
+      <c r="BR14" t="s">
+        <v>148</v>
+      </c>
+      <c r="BZ14">
+        <v>39396</v>
+      </c>
+      <c r="CB14">
+        <v>0</v>
+      </c>
+      <c r="CC14">
+        <v>2</v>
+      </c>
+      <c r="CD14" t="s">
+        <v>149</v>
+      </c>
+      <c r="CE14" t="s">
+        <v>150</v>
+      </c>
+      <c r="CG14">
+        <v>37</v>
+      </c>
+      <c r="CH14" t="s">
+        <v>151</v>
+      </c>
+      <c r="CI14" t="s">
+        <v>152</v>
+      </c>
+      <c r="CJ14" t="b">
+        <v>1</v>
+      </c>
+      <c r="CK14">
+        <v>13.148</v>
+      </c>
+      <c r="CL14" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="15" spans="1:96">
+      <c r="A15" s="1">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D15" t="s">
+        <v>97</v>
+      </c>
+      <c r="E15" t="s">
+        <v>98</v>
+      </c>
+      <c r="F15" t="s">
+        <v>99</v>
+      </c>
+      <c r="H15">
+        <v>980181</v>
+      </c>
+      <c r="J15">
+        <v>194</v>
+      </c>
+      <c r="K15" t="s">
+        <v>100</v>
+      </c>
+      <c r="L15">
+        <v>46356674</v>
+      </c>
+      <c r="M15" t="s">
+        <v>101</v>
+      </c>
+      <c r="N15">
+        <v>35.136722</v>
+      </c>
+      <c r="O15">
+        <v>-89.945753</v>
+      </c>
+      <c r="P15">
+        <v>46344</v>
+      </c>
+      <c r="Q15">
+        <v>201</v>
+      </c>
+      <c r="R15">
+        <v>170</v>
+      </c>
+      <c r="S15" t="s">
+        <v>107</v>
+      </c>
+      <c r="T15" t="s">
+        <v>111</v>
+      </c>
+      <c r="U15">
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>30.9</v>
+      </c>
+      <c r="X15">
+        <v>4</v>
+      </c>
+      <c r="Y15">
+        <v>4</v>
+      </c>
+      <c r="Z15" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA15">
+        <v>29.5</v>
+      </c>
+      <c r="AB15">
+        <v>0</v>
+      </c>
+      <c r="AF15">
+        <v>2</v>
+      </c>
+      <c r="AG15">
+        <v>0</v>
+      </c>
+      <c r="AH15">
+        <v>3</v>
+      </c>
+      <c r="AI15">
+        <v>7</v>
+      </c>
+      <c r="AJ15">
+        <v>6</v>
+      </c>
+      <c r="AK15">
+        <v>0</v>
+      </c>
+      <c r="AL15">
+        <v>12</v>
+      </c>
+      <c r="AM15">
+        <v>3</v>
+      </c>
+      <c r="AN15">
+        <v>3</v>
+      </c>
+      <c r="AO15" t="s">
+        <v>114</v>
+      </c>
+      <c r="AP15" t="s">
+        <v>128</v>
+      </c>
+      <c r="AQ15" t="s">
+        <v>130</v>
+      </c>
+      <c r="AS15">
+        <v>47157</v>
+      </c>
+      <c r="AT15">
+        <v>4</v>
+      </c>
+      <c r="AU15" t="s">
+        <v>131</v>
+      </c>
+      <c r="AV15">
+        <v>0</v>
+      </c>
+      <c r="AW15" t="s">
+        <v>133</v>
+      </c>
+      <c r="AX15" t="s">
+        <v>139</v>
+      </c>
+      <c r="AY15" t="s">
+        <v>133</v>
+      </c>
+      <c r="AZ15" t="s">
+        <v>142</v>
+      </c>
+      <c r="BC15" t="s">
+        <v>145</v>
+      </c>
+      <c r="BF15">
+        <v>267466</v>
+      </c>
+      <c r="BG15" t="s">
+        <v>146</v>
+      </c>
+      <c r="BM15" t="s">
+        <v>147</v>
+      </c>
+      <c r="BR15" t="s">
+        <v>148</v>
+      </c>
+      <c r="BZ15">
+        <v>39396</v>
+      </c>
+      <c r="CB15">
+        <v>0</v>
+      </c>
+      <c r="CC15">
+        <v>3</v>
+      </c>
+      <c r="CD15" t="s">
+        <v>149</v>
+      </c>
+      <c r="CE15" t="s">
+        <v>150</v>
+      </c>
+      <c r="CG15">
+        <v>37</v>
+      </c>
+      <c r="CH15" t="s">
+        <v>151</v>
+      </c>
+      <c r="CI15" t="s">
+        <v>152</v>
+      </c>
+      <c r="CJ15" t="b">
+        <v>1</v>
+      </c>
+      <c r="CK15">
+        <v>13.148</v>
+      </c>
+      <c r="CL15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="16" spans="1:96">
+      <c r="A16" s="1">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" t="s">
+        <v>96</v>
+      </c>
+      <c r="D16" t="s">
+        <v>97</v>
+      </c>
+      <c r="E16" t="s">
+        <v>98</v>
+      </c>
+      <c r="F16" t="s">
+        <v>99</v>
+      </c>
+      <c r="H16">
+        <v>980181</v>
+      </c>
+      <c r="J16">
+        <v>201</v>
+      </c>
+      <c r="K16" t="s">
+        <v>100</v>
+      </c>
+      <c r="L16">
+        <v>46356681</v>
+      </c>
+      <c r="M16" t="s">
+        <v>101</v>
+      </c>
+      <c r="N16">
+        <v>35.136722</v>
+      </c>
+      <c r="O16">
+        <v>-89.945753</v>
+      </c>
+      <c r="P16">
+        <v>46344</v>
+      </c>
+      <c r="Q16">
+        <v>202</v>
+      </c>
+      <c r="R16">
+        <v>170</v>
+      </c>
+      <c r="S16" t="s">
+        <v>107</v>
+      </c>
+      <c r="T16" t="s">
+        <v>108</v>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <v>30.9</v>
+      </c>
+      <c r="X16">
+        <v>4</v>
+      </c>
+      <c r="Y16">
+        <v>4</v>
+      </c>
+      <c r="Z16" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA16">
+        <v>29.5</v>
+      </c>
+      <c r="AB16">
+        <v>120</v>
+      </c>
+      <c r="AF16">
+        <v>2</v>
+      </c>
+      <c r="AG16">
+        <v>1</v>
+      </c>
+      <c r="AH16">
+        <v>0</v>
+      </c>
+      <c r="AI16">
+        <v>8</v>
+      </c>
+      <c r="AJ16">
+        <v>8</v>
+      </c>
+      <c r="AK16">
+        <v>0</v>
+      </c>
+      <c r="AL16">
+        <v>12</v>
+      </c>
+      <c r="AM16">
+        <v>4</v>
+      </c>
+      <c r="AN16">
+        <v>4</v>
+      </c>
+      <c r="AO16" t="s">
+        <v>114</v>
+      </c>
+      <c r="AP16" t="s">
+        <v>129</v>
+      </c>
+      <c r="AQ16" t="s">
+        <v>130</v>
+      </c>
+      <c r="AS16">
+        <v>47157</v>
+      </c>
+      <c r="AT16">
+        <v>4</v>
+      </c>
+      <c r="AU16" t="s">
+        <v>131</v>
+      </c>
+      <c r="AV16">
+        <v>0</v>
+      </c>
+      <c r="AW16" t="s">
+        <v>133</v>
+      </c>
+      <c r="AX16" t="s">
+        <v>139</v>
+      </c>
+      <c r="AY16" t="s">
+        <v>133</v>
+      </c>
+      <c r="AZ16" t="s">
+        <v>142</v>
+      </c>
+      <c r="BC16" t="s">
+        <v>145</v>
+      </c>
+      <c r="BF16">
+        <v>267466</v>
+      </c>
+      <c r="BG16" t="s">
+        <v>146</v>
+      </c>
+      <c r="BM16" t="s">
+        <v>147</v>
+      </c>
+      <c r="BR16" t="s">
+        <v>148</v>
+      </c>
+      <c r="BZ16">
+        <v>39396</v>
+      </c>
+      <c r="CB16">
+        <v>1</v>
+      </c>
+      <c r="CC16">
+        <v>0</v>
+      </c>
+      <c r="CD16" t="s">
+        <v>149</v>
+      </c>
+      <c r="CE16" t="s">
+        <v>150</v>
+      </c>
+      <c r="CG16">
+        <v>37</v>
+      </c>
+      <c r="CH16" t="s">
+        <v>151</v>
+      </c>
+      <c r="CI16" t="s">
+        <v>152</v>
+      </c>
+      <c r="CJ16" t="b">
+        <v>1</v>
+      </c>
+      <c r="CK16">
+        <v>13.148</v>
+      </c>
+      <c r="CL16" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>